<commit_message>
redistribucion del ultimo grupo
</commit_message>
<xml_diff>
--- a/b_2023_2_GIT (lista de grupos).xlsx
+++ b/b_2023_2_GIT (lista de grupos).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogerruizescobar/Documents/2023-1_Sistemas de Infromacion y Sistemas Inteligentes/2023-2/Grupo B/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogerruizescobar/Documents/2023-1_Sistemas de Infromacion y Sistemas Inteligentes/2023-2/Grupo B/UDABOL/UDABOL_2023-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9432882C-99B3-8844-BB6F-86C0A6732D8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD17A4E7-B1D8-954F-9308-D3FC97E0F816}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14400" xr2:uid="{A6C412E0-E981-AD4F-9D3B-4CC9DB6BD680}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14320" xr2:uid="{A6C412E0-E981-AD4F-9D3B-4CC9DB6BD680}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -489,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4300398C-630E-364C-8255-E9949C520F5E}">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -573,7 +573,7 @@
         <v>#N/A</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -643,7 +643,7 @@
         <v>#N/A</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -713,7 +713,7 @@
         <v>#N/A</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -783,7 +783,7 @@
         <v>57938</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -853,7 +853,7 @@
         <v>59923</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -923,7 +923,7 @@
         <v>#N/A</v>
       </c>
       <c r="D31">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -993,7 +993,7 @@
         <v>#N/A</v>
       </c>
       <c r="D36">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:1">

</xml_diff>

<commit_message>
Se adiciono el proyecto
</commit_message>
<xml_diff>
--- a/b_2023_2_GIT (lista de grupos).xlsx
+++ b/b_2023_2_GIT (lista de grupos).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogerruizescobar/Documents/2023-1_Sistemas de Infromacion y Sistemas Inteligentes/2023-2/Grupo B/UDABOL/UDABOL_2023-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogerruizescobar/Documents/2023-1_Sistemas de Infromacion y Sistemas Inteligentes/2023-2/Grupo B/UDABOL_2023-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4477004A-2709-054A-AF05-D54EF13E5C7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7174FE48-FC33-B54B-9062-E2C9438CAD2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{A6C412E0-E981-AD4F-9D3B-4CC9DB6BD680}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14400" xr2:uid="{A6C412E0-E981-AD4F-9D3B-4CC9DB6BD680}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Nombres</t>
   </si>
@@ -136,16 +136,13 @@
   </si>
   <si>
     <t>BARRIENTOS CUELLAR CUELLAR WILSON</t>
-  </si>
-  <si>
-    <t>BLANCO CADENA HUASCAR ELIAS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -492,16 +489,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4300398C-630E-364C-8255-E9949C520F5E}">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="38.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -509,7 +506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -523,7 +520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -537,7 +534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -551,7 +548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -565,7 +562,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -579,7 +576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -590,10 +587,10 @@
         <v>59883</v>
       </c>
       <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -604,10 +601,10 @@
         <v>#N/A</v>
       </c>
       <c r="D8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -618,10 +615,10 @@
         <v>#N/A</v>
       </c>
       <c r="D9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -632,10 +629,10 @@
         <v>#N/A</v>
       </c>
       <c r="D10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -649,7 +646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -660,10 +657,10 @@
         <v>67279</v>
       </c>
       <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -674,10 +671,10 @@
         <v>#N/A</v>
       </c>
       <c r="D13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -688,10 +685,10 @@
         <v>#N/A</v>
       </c>
       <c r="D14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -702,10 +699,10 @@
         <v>#N/A</v>
       </c>
       <c r="D15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>15</v>
       </c>
@@ -719,7 +716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -730,10 +727,10 @@
         <v>57756</v>
       </c>
       <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -744,10 +741,10 @@
         <v>#N/A</v>
       </c>
       <c r="D18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
@@ -758,10 +755,10 @@
         <v>#N/A</v>
       </c>
       <c r="D19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -772,10 +769,10 @@
         <v>56352</v>
       </c>
       <c r="D20">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -789,7 +786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>21</v>
       </c>
@@ -803,7 +800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>22</v>
       </c>
@@ -817,7 +814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>23</v>
       </c>
@@ -831,7 +828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>24</v>
       </c>
@@ -845,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>25</v>
       </c>
@@ -859,7 +856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>26</v>
       </c>
@@ -870,10 +867,10 @@
         <v>58201</v>
       </c>
       <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>27</v>
       </c>
@@ -884,10 +881,10 @@
         <v>#N/A</v>
       </c>
       <c r="D28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>28</v>
       </c>
@@ -898,10 +895,10 @@
         <v>#N/A</v>
       </c>
       <c r="D29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>29</v>
       </c>
@@ -912,10 +909,10 @@
         <v>68439</v>
       </c>
       <c r="D30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>30</v>
       </c>
@@ -929,7 +926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>31</v>
       </c>
@@ -940,10 +937,10 @@
         <v>#N/A</v>
       </c>
       <c r="D32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>32</v>
       </c>
@@ -954,10 +951,10 @@
         <v>#N/A</v>
       </c>
       <c r="D33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>33</v>
       </c>
@@ -968,10 +965,10 @@
         <v>#N/A</v>
       </c>
       <c r="D34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>34</v>
       </c>
@@ -982,10 +979,10 @@
         <v>#N/A</v>
       </c>
       <c r="D35">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>35</v>
       </c>
@@ -999,155 +996,147 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1">
       <c r="A50">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1">
       <c r="A51">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1">
       <c r="A52">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1">
       <c r="A53">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1">
       <c r="A54">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1">
       <c r="A55">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1">
       <c r="A56">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1">
       <c r="A57">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1">
       <c r="A58">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1">
       <c r="A59">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1">
       <c r="A60">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1">
       <c r="A61">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1">
       <c r="A62">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1">
       <c r="A63">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1">
       <c r="A64">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1">
       <c r="A65">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1">
       <c r="A66">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1">
       <c r="A67">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1">
       <c r="A68">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1">
       <c r="A69">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1">
       <c r="A70">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1">
       <c r="A71">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1">
       <c r="A72">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1">
       <c r="A73">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1">
       <c r="A74">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1">
       <c r="A75">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1">
       <c r="A76">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1">
       <c r="A77">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1">
       <c r="A78">
         <v>77</v>
       </c>

</xml_diff>